<commit_message>
Integration HTML tests are added to the appendix and database folder is added
</commit_message>
<xml_diff>
--- a/Documentation/5 - Test/TestCaseTests.xlsx
+++ b/Documentation/5 - Test/TestCaseTests.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karrt\Desktop\All_Folders\Uni\Semester3\Semester Project Heterogeneous System (SEP3)\1 SEP3\SEP3XA20-ARS\Documentations\5 - Test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karrt\Desktop\All_Folders\Uni\Semester3\Semester Project Heterogeneous System (SEP3)\1 SEP3\SEP3XA20-ARS\Documentation\5 - Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C511573B-B7CB-430A-A3A3-CF51B8F98150}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6B5BA2F-66C7-4614-8446-EFE105B9ACB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{DEFFF7F6-8050-4346-AF45-C0EFE5BA9B6C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="49">
   <si>
     <t>Requirement
 ID</t>
@@ -181,6 +181,69 @@
   </si>
   <si>
     <t>Check Customer's editing of user information with valid data</t>
+  </si>
+  <si>
+    <t>1. Click on 'Register Here'
+2. Enter first name
+3. Enter last name
+4. Enter phone number
+5. Enter birthdate
+6. Enter email
+7. Enter password</t>
+  </si>
+  <si>
+    <t>first name = Ben
+last name = Dover
+phone number = 123456789
+birthdate = 22-01-1993
+email = customer@gmail.com
+password = customer</t>
+  </si>
+  <si>
+    <t>first name = Ben
+last name = Dover
+phone number = 12345678910
+birthdate = 22-01-2500
+email = customer
+password = 123</t>
+  </si>
+  <si>
+    <t>Register should not be successful and there should be specific error messages saying what is wrong</t>
+  </si>
+  <si>
+    <t>user is registered
+ and user information 
+is stored in the 
+database</t>
+  </si>
+  <si>
+    <t>1. Click on 'Edit Profile' found under 'My Profile'
+2. Enter first name
+3. Enter last name
+4. Enter phone number
+5. Enter birthdate
+6. Enter email
+7. Enter password</t>
+  </si>
+  <si>
+    <t>first name = Saul
+last name = T. Nutz
+phone number = 987654321
+birthdate = 22-01-1994
+email = customer1@gmail.com
+password = customer1</t>
+  </si>
+  <si>
+    <t>User info is changed</t>
+  </si>
+  <si>
+    <t>(The same information as when registered or previously changed)
+first name = Ben
+last name = Dover
+phone number = 123456789
+birthdate = 22-01-1993
+email = customer@gmail.com
+password = customer</t>
   </si>
 </sst>
 </file>
@@ -538,7 +601,7 @@
   <dimension ref="B2:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -547,7 +610,7 @@
     <col min="3" max="3" width="11.54296875" customWidth="1"/>
     <col min="4" max="5" width="13.1796875" customWidth="1"/>
     <col min="6" max="6" width="15.26953125" customWidth="1"/>
-    <col min="7" max="7" width="25.453125" customWidth="1"/>
+    <col min="7" max="7" width="28" customWidth="1"/>
     <col min="8" max="8" width="12.453125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -580,7 +643,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="2:10" ht="116" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:10" ht="188.5" x14ac:dyDescent="0.35">
       <c r="B3">
         <v>1</v>
       </c>
@@ -593,7 +656,12 @@
       <c r="E3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="1"/>
+      <c r="F3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="H3" s="1" t="s">
         <v>10</v>
       </c>
@@ -604,7 +672,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="2:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:10" ht="188.5" x14ac:dyDescent="0.35">
       <c r="B4">
         <v>2</v>
       </c>
@@ -616,6 +684,21 @@
       </c>
       <c r="E4" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="72.5" x14ac:dyDescent="0.35">
@@ -816,7 +899,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:10" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B17">
         <v>15</v>
       </c>
@@ -824,7 +907,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="2:4" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:10" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B18">
         <v>16</v>
       </c>
@@ -832,20 +915,56 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="2:4" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:10" ht="217.5" x14ac:dyDescent="0.35">
       <c r="B19">
         <v>17</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="E19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" ht="217.5" x14ac:dyDescent="0.35">
       <c r="B20">
         <v>18</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>39</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Process report - Intro, Project description, execution, critique and supervision
</commit_message>
<xml_diff>
--- a/Documentation/5 - Test/TestCaseTests.xlsx
+++ b/Documentation/5 - Test/TestCaseTests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karrt\Desktop\All_Folders\Uni\Semester3\Semester Project Heterogeneous System (SEP3)\1 SEP3\SEP3XA20-ARS\Documentation\5 - Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6B5BA2F-66C7-4614-8446-EFE105B9ACB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2215F60-4CF4-41EE-A469-50590DD1D658}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{DEFFF7F6-8050-4346-AF45-C0EFE5BA9B6C}"/>
   </bookViews>
@@ -34,11 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="49">
-  <si>
-    <t>Requirement
-ID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="82">
   <si>
     <t>Test Scenario</t>
   </si>
@@ -153,9 +149,6 @@
     <t>Check the creation of flights by the Operator with invalid data</t>
   </si>
   <si>
-    <t>3, 4</t>
-  </si>
-  <si>
     <t>Check searching of flights to view available flights with valid data</t>
   </si>
   <si>
@@ -175,9 +168,6 @@
   </si>
   <si>
     <t>Check whether the Operator can delay a flight with valid data</t>
-  </si>
-  <si>
-    <t>1, 2, 9, 11, 17</t>
   </si>
   <si>
     <t>Check Customer's editing of user information with valid data</t>
@@ -245,13 +235,211 @@
 email = customer@gmail.com
 password = customer</t>
   </si>
+  <si>
+    <t>Operator is logged in and the airports and airplanes are stored in the database</t>
+  </si>
+  <si>
+    <t>1. Choose the departure airport
+2. Choose the arrival airport
+3. Set the departure date and time
+4. Set the arrival date and time
+5. Choose the airplane</t>
+  </si>
+  <si>
+    <t>departure airport = Copenhagen Airport
+arrival airport = Singapor Changi Airport
+departure date = 10/12/2020
+departure time = 13:00
+arrival date = 11/12/2020
+arrival time = 09:00
+Airplane = Boeing 737</t>
+  </si>
+  <si>
+    <t>Flight is added and should be visisble to operator and customer</t>
+  </si>
+  <si>
+    <t>the invalid data here is that the dates are in the past
+departure airport = Copenhagen Airport
+arrival airport = Singapor Changi Airport
+departure date = 02/12/2020
+departure time = 13:00
+arrival date = 03/12/2020
+arrival time = 09:00
+Airplane = Boeing 737</t>
+  </si>
+  <si>
+    <t>An error should be shown and the flight should not be added</t>
+  </si>
+  <si>
+    <t>User is logged in and at least one flight is added to the database</t>
+  </si>
+  <si>
+    <t>1. Choose the departure airport
+2. Choose the arrival airport
+3. Set the departure date
+4. Enter the number tickets for adults and children</t>
+  </si>
+  <si>
+    <t>departure airport = Copenhagen Airport
+arrival airport = Singapor Changi Airport
+departure date = 10/12/2020
+number of adults  =  2
+number of children = 1</t>
+  </si>
+  <si>
+    <t>Available flights on that date should be shown</t>
+  </si>
+  <si>
+    <t>the invalid data here is that the deparature date is in the past
+departure airport = Copenhagen Airport
+arrival airport = Singapor Changi Airport
+departure date = 02/12/2020
+number of adults  =  2
+number of children = 1</t>
+  </si>
+  <si>
+    <t>An error asking for a valid date will be shown</t>
+  </si>
+  <si>
+    <t>User is logged in and search an available flight to book</t>
+  </si>
+  <si>
+    <t>1. Click on book for the searched flight
+2. Enter first name
+3 Enter last name
+4. Pick a gender
+5. Enter date of birth of the passenger
+6. Enter nationality of the passenger
+7. Enter the passport number
+8. Enter the passport expiration date
+9. Click on continue
+10. Pick the luggage option
+11. Select a seat to reserve
+12. Enter name on credit card
+13. Enter credit card number
+14. Enter CVV
+15. Enter credit card's expiration month and year
+16. Click on Pay</t>
+  </si>
+  <si>
+    <t>first name = Geralt
+last name = Of Rivia
+gender = M
+date of birth = 12/12/1990
+nationality = Polish
+passport number = 1234567891
+passport expiration date = 01/01/2025
+luggage = small
+seat number = 1D
+name on credit card = Geralt Of Rivia
+credit card number = 1234567891234567
+CVV = 333
+expiration month = 05
+expiration year = 2024</t>
+  </si>
+  <si>
+    <t>The flight should be booked by the user and a code ticket will be returned to the user</t>
+  </si>
+  <si>
+    <t>the invalid data here is that this passenger has the same passport number as another passenger on the same flight, the brithdate is in the future, selecting an already reserved seat, and invalid inputs
+first name = Geralt
+last name = Of Rivia
+gender = M
+date of birth = 12/12/1990
+nationality = Polish
+passport number = 1234567891
+passport expiration date = 01/01/2025
+luggage = small
+seat number = 1D
+name on credit card = Geralt Of Rivia
+credit card number = 1234567891234567
+CVV = 333
+expiration month = 05
+expiration year = 2024</t>
+  </si>
+  <si>
+    <t>Errors with specific error messages will shown to inform the user what went wrong</t>
+  </si>
+  <si>
+    <t>User has already booked a flight</t>
+  </si>
+  <si>
+    <t>1. Go to Overview, found under My Profile
+2. Click on View Details for the ticket that is about to be cancelled
+3. Click on Cancel Flight</t>
+  </si>
+  <si>
+    <t>not relevant</t>
+  </si>
+  <si>
+    <t>The booked flight is cancelled and the reserved seat will be available for other users to reserve</t>
+  </si>
+  <si>
+    <t>Check whether users can log out</t>
+  </si>
+  <si>
+    <t>user is logged
+ in</t>
+  </si>
+  <si>
+    <t>1. Click the log
+ out button</t>
+  </si>
+  <si>
+    <t>user is logged out</t>
+  </si>
+  <si>
+    <t>The about to be delayed flight is created by the operator and stored in the database</t>
+  </si>
+  <si>
+    <t>1. Got to Manage Flights
+2. Click on Delay Flight on the desired flight
+3. Enter how many hours and minutes the flight should be delayed
+4. Click on Confirm</t>
+  </si>
+  <si>
+    <t>hours = 10
+minutes = 36</t>
+  </si>
+  <si>
+    <t>The flight has been delayed by 10 hours and 36 minutes, and the customers who have booked the flight should get a notification</t>
+  </si>
+  <si>
+    <t>The about to be cancelled flight is created by the operator and stored in the database</t>
+  </si>
+  <si>
+    <t>1. Go to Manage Flights
+2. Click on Cancel Flight on the desired flight
+3. Click on confirm</t>
+  </si>
+  <si>
+    <t>The chosen flight is cancelled and customers who have booked the cancelled flight will get a notification</t>
+  </si>
+  <si>
+    <t>Check whether the Operator can delay a flight with invalid data</t>
+  </si>
+  <si>
+    <t>hours = -10
+minutes = Thirty-six</t>
+  </si>
+  <si>
+    <t>Error message will be shown</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -279,11 +467,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -598,10 +790,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC4BB4D1-8408-4829-AEAA-064C216F932E}">
-  <dimension ref="B2:J20"/>
+  <dimension ref="B2:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -614,99 +806,90 @@
     <col min="8" max="8" width="12.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="2:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="G2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="2:10" ht="188.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="2:9" ht="188.5" x14ac:dyDescent="0.35">
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="H3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" ht="188.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="2:9" ht="188.5" x14ac:dyDescent="0.35">
       <c r="B4">
         <v>2</v>
       </c>
-      <c r="C4">
-        <v>7</v>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="H4" s="1" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10" ht="72.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="2:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B5">
         <v>3</v>
       </c>
-      <c r="C5">
-        <v>8</v>
+      <c r="C5" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>15</v>
@@ -721,24 +904,21 @@
         <v>18</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J5" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" ht="87" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="2:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B6">
         <v>4</v>
       </c>
-      <c r="C6">
-        <v>8</v>
+      <c r="C6" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>16</v>
@@ -747,227 +927,407 @@
         <v>17</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" ht="72.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="2:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B7">
         <v>5</v>
       </c>
-      <c r="C7">
-        <v>15</v>
+      <c r="C7" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>23</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J7" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10" ht="87" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="2:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B8">
         <v>6</v>
       </c>
-      <c r="C8">
-        <v>15</v>
+      <c r="C8" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="H8" s="1" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J8" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" ht="72.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="2:9" ht="246.5" x14ac:dyDescent="0.35">
       <c r="B9">
         <v>7</v>
       </c>
-      <c r="C9">
-        <v>12</v>
+      <c r="C9" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" ht="72.5" x14ac:dyDescent="0.35">
+        <v>46</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" ht="319" x14ac:dyDescent="0.35">
       <c r="B10">
         <v>8</v>
       </c>
-      <c r="C10">
-        <v>12</v>
+      <c r="C10" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10" ht="87" x14ac:dyDescent="0.35">
+        <v>46</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" ht="188.5" x14ac:dyDescent="0.35">
       <c r="B11">
         <v>9</v>
       </c>
-      <c r="C11" t="s">
-        <v>30</v>
+      <c r="C11" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10" ht="87" x14ac:dyDescent="0.35">
+        <v>52</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" ht="261" x14ac:dyDescent="0.35">
       <c r="B12">
         <v>10</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="B13">
+        <v>11</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="B14">
+        <v>12</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="13" spans="2:10" ht="58" x14ac:dyDescent="0.35">
-      <c r="B13">
-        <v>11</v>
-      </c>
-      <c r="C13" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" ht="58" x14ac:dyDescent="0.35">
-      <c r="B14">
-        <v>12</v>
-      </c>
-      <c r="C14" t="s">
-        <v>38</v>
-      </c>
       <c r="D14" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10" ht="72.5" x14ac:dyDescent="0.35">
+        <v>58</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" ht="174" x14ac:dyDescent="0.35">
       <c r="B15">
         <v>13</v>
       </c>
+      <c r="C15" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="D15" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10" ht="58" x14ac:dyDescent="0.35">
+        <v>64</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" ht="130.5" x14ac:dyDescent="0.35">
       <c r="B16">
         <v>14</v>
       </c>
+      <c r="C16" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="D16" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" ht="72.5" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" ht="217.5" x14ac:dyDescent="0.35">
       <c r="B17">
         <v>15</v>
       </c>
+      <c r="C17" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="D17" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" ht="72.5" x14ac:dyDescent="0.35">
+        <v>72</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" ht="217.5" x14ac:dyDescent="0.35">
       <c r="B18">
         <v>16</v>
       </c>
+      <c r="C18" s="1" t="s">
+        <v>79</v>
+      </c>
       <c r="D18" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" ht="217.5" x14ac:dyDescent="0.35">
+        <v>72</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" ht="217.5" x14ac:dyDescent="0.35">
       <c r="B19">
         <v>17</v>
       </c>
+      <c r="C19" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="D19" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="H19" s="1" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J19" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" ht="217.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="2:9" ht="261" x14ac:dyDescent="0.35">
       <c r="B20">
         <v>18</v>
       </c>
+      <c r="C20" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="D20" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>45</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J20" s="1" t="s">
-        <v>13</v>
+    </row>
+    <row r="21" spans="2:9" ht="58" x14ac:dyDescent="0.35">
+      <c r="B21">
+        <v>19</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>